<commit_message>
add new ket quả a Văn gửi hệ số
</commit_message>
<xml_diff>
--- a/hồ sơ/chấm điểm_TD_T8.xlsx
+++ b/hồ sơ/chấm điểm_TD_T8.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="204">
   <si>
     <t>Họ Tên</t>
   </si>
@@ -658,6 +658,15 @@
   </si>
   <si>
     <t>a Văn chấm 85</t>
+  </si>
+  <si>
+    <t>Kết Quả Đợt 1</t>
+  </si>
+  <si>
+    <t>Tuyển</t>
+  </si>
+  <si>
+    <t>Không Tuyển</t>
   </si>
 </sst>
 </file>
@@ -748,7 +757,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,6 +797,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,7 +909,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1106,6 +1121,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1114,6 +1132,14 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1399,50 +1425,54 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="15" max="15" width="21" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="87" t="s">
+      <c r="C1" s="89"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="87" t="s">
+      <c r="F1" s="89"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="88" t="s">
         <v>187</v>
       </c>
-      <c r="I1" s="88"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="87" t="s">
+      <c r="I1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="88"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="56" t="s">
+      <c r="L1" s="89"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="87" t="s">
+        <v>201</v>
+      </c>
+      <c r="O1" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="56" t="s">
+      <c r="P1" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="79"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77"/>
@@ -1482,12 +1512,12 @@
       <c r="M2" s="82" t="s">
         <v>194</v>
       </c>
-      <c r="N2" s="22"/>
+      <c r="N2" s="82"/>
       <c r="O2" s="22"/>
-      <c r="P2" s="54"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="91" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="85">
@@ -1523,18 +1553,18 @@
         <f>D3+G3+J3</f>
         <v>0</v>
       </c>
-      <c r="N3" s="54" t="s">
+      <c r="N3" s="94" t="s">
+        <v>202</v>
+      </c>
+      <c r="O3" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="P3" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="P3" s="80" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="91" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="85">
@@ -1559,27 +1589,29 @@
       </c>
       <c r="J4" s="83"/>
       <c r="K4" s="85">
-        <f t="shared" ref="K4:K31" si="0">B4+E4+H4</f>
+        <f t="shared" ref="K4:K28" si="0">B4+E4+H4</f>
         <v>72</v>
       </c>
       <c r="L4" s="81">
-        <f t="shared" ref="L4:L31" si="1">C4+F4+I4</f>
+        <f t="shared" ref="L4:L28" si="1">C4+F4+I4</f>
         <v>72</v>
       </c>
       <c r="M4" s="83">
-        <f t="shared" ref="M4:M31" si="2">D4+G4+J4</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="54" t="s">
+        <f t="shared" ref="M4:M28" si="2">D4+G4+J4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="94" t="s">
+        <v>202</v>
+      </c>
+      <c r="O4" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="O4" s="57" t="s">
+      <c r="P4" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="P4" s="80"/>
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="92" t="s">
         <v>149</v>
       </c>
       <c r="B5" s="85">
@@ -1615,129 +1647,173 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N5" s="54" t="s">
+      <c r="N5" s="94" t="s">
+        <v>202</v>
+      </c>
+      <c r="O5" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="O5" s="57" t="s">
+      <c r="P5" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="P5" s="80"/>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="74" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="83"/>
+      <c r="A6" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="85">
+        <v>40</v>
+      </c>
+      <c r="C6" s="81">
+        <v>43</v>
+      </c>
+      <c r="D6" s="83">
+        <v>45</v>
+      </c>
+      <c r="E6" s="85">
+        <v>15</v>
+      </c>
+      <c r="F6" s="81">
+        <v>12</v>
+      </c>
+      <c r="G6" s="83">
+        <v>8</v>
+      </c>
+      <c r="H6" s="85">
+        <v>12</v>
+      </c>
+      <c r="I6" s="81">
+        <v>15</v>
+      </c>
+      <c r="J6" s="83">
+        <v>9</v>
+      </c>
       <c r="K6" s="85">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B6+E6+H6</f>
+        <v>67</v>
       </c>
       <c r="L6" s="81">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C6+F6+I6</f>
+        <v>70</v>
       </c>
       <c r="M6" s="83">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="57" t="s">
-        <v>167</v>
-      </c>
-      <c r="O6" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="P6" s="80"/>
+        <f>D6+G6+J6</f>
+        <v>62</v>
+      </c>
+      <c r="N6" s="94" t="s">
+        <v>202</v>
+      </c>
+      <c r="O6" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="P6" s="57" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="85"/>
+      <c r="A7" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="85">
+        <v>40</v>
+      </c>
       <c r="C7" s="81"/>
       <c r="D7" s="83"/>
-      <c r="E7" s="85"/>
+      <c r="E7" s="85">
+        <v>7</v>
+      </c>
       <c r="F7" s="81"/>
       <c r="G7" s="83"/>
-      <c r="H7" s="85"/>
+      <c r="H7" s="85">
+        <v>7</v>
+      </c>
       <c r="I7" s="81"/>
       <c r="J7" s="83"/>
       <c r="K7" s="85">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B7+E7+H7</f>
+        <v>54</v>
       </c>
       <c r="L7" s="81">
-        <f t="shared" si="1"/>
+        <f>C7+F7+I7</f>
         <v>0</v>
       </c>
       <c r="M7" s="83">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="57" t="s">
-        <v>167</v>
+        <f>D7+G7+J7</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="94" t="s">
+        <v>202</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="P7" s="80"/>
+        <v>138</v>
+      </c>
+      <c r="P7" s="57" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="85"/>
+      <c r="A8" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="85">
+        <v>50</v>
+      </c>
       <c r="C8" s="81"/>
       <c r="D8" s="83"/>
-      <c r="E8" s="85"/>
+      <c r="E8" s="85">
+        <v>10</v>
+      </c>
       <c r="F8" s="81"/>
       <c r="G8" s="83"/>
-      <c r="H8" s="85"/>
+      <c r="H8" s="85">
+        <v>5</v>
+      </c>
       <c r="I8" s="81"/>
       <c r="J8" s="83"/>
       <c r="K8" s="85">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B8+E8+H8</f>
+        <v>65</v>
       </c>
       <c r="L8" s="81">
-        <f t="shared" si="1"/>
+        <f>C8+F8+I8</f>
         <v>0</v>
       </c>
       <c r="M8" s="83">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="57" t="s">
+        <f>D8+G8+J8</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="94" t="s">
+        <v>202</v>
+      </c>
+      <c r="O8" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="O8" s="57" t="s">
+      <c r="P8" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="P8" s="80"/>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="85"/>
+      <c r="A9" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="85">
+        <v>50</v>
+      </c>
       <c r="C9" s="81"/>
       <c r="D9" s="83"/>
-      <c r="E9" s="85"/>
+      <c r="E9" s="85">
+        <v>10</v>
+      </c>
       <c r="F9" s="81"/>
       <c r="G9" s="83"/>
-      <c r="H9" s="85"/>
+      <c r="H9" s="85">
+        <v>5</v>
+      </c>
       <c r="I9" s="81"/>
       <c r="J9" s="83"/>
       <c r="K9" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="L9" s="81">
         <f t="shared" si="1"/>
@@ -1747,30 +1823,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N9" s="54" t="s">
-        <v>138</v>
+      <c r="N9" s="94" t="s">
+        <v>202</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="P9" s="80"/>
+        <v>167</v>
+      </c>
+      <c r="P9" s="57" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="85"/>
+        <v>28</v>
+      </c>
+      <c r="B10" s="85">
+        <v>20</v>
+      </c>
       <c r="C10" s="81"/>
       <c r="D10" s="83"/>
-      <c r="E10" s="85"/>
+      <c r="E10" s="85">
+        <v>10</v>
+      </c>
       <c r="F10" s="81"/>
       <c r="G10" s="83"/>
-      <c r="H10" s="85"/>
+      <c r="H10" s="85">
+        <v>10</v>
+      </c>
       <c r="I10" s="81"/>
       <c r="J10" s="83"/>
       <c r="K10" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L10" s="81">
         <f t="shared" si="1"/>
@@ -1780,30 +1864,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N10" s="54" t="s">
-        <v>138</v>
+      <c r="N10" s="80" t="s">
+        <v>203</v>
       </c>
       <c r="O10" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="P10" s="80"/>
+        <v>167</v>
+      </c>
+      <c r="P10" s="57" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="85"/>
+        <v>58</v>
+      </c>
+      <c r="B11" s="85">
+        <v>35</v>
+      </c>
       <c r="C11" s="81"/>
       <c r="D11" s="83"/>
-      <c r="E11" s="85"/>
+      <c r="E11" s="85">
+        <v>7</v>
+      </c>
       <c r="F11" s="81"/>
       <c r="G11" s="83"/>
-      <c r="H11" s="85"/>
+      <c r="H11" s="85">
+        <v>10</v>
+      </c>
       <c r="I11" s="81"/>
       <c r="J11" s="83"/>
       <c r="K11" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="L11" s="81">
         <f t="shared" si="1"/>
@@ -1813,30 +1905,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N11" s="54" t="s">
+      <c r="N11" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O11" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="O11" s="57" t="s">
+      <c r="P11" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="P11" s="80"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="85"/>
+        <v>71</v>
+      </c>
+      <c r="B12" s="85">
+        <v>20</v>
+      </c>
       <c r="C12" s="81"/>
       <c r="D12" s="83"/>
-      <c r="E12" s="85"/>
+      <c r="E12" s="85">
+        <v>10</v>
+      </c>
       <c r="F12" s="81"/>
       <c r="G12" s="83"/>
-      <c r="H12" s="85"/>
+      <c r="H12" s="85">
+        <v>10</v>
+      </c>
       <c r="I12" s="81"/>
       <c r="J12" s="83"/>
       <c r="K12" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L12" s="81">
         <f t="shared" si="1"/>
@@ -1846,30 +1946,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N12" s="54" t="s">
+      <c r="N12" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O12" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="O12" s="57" t="s">
+      <c r="P12" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="P12" s="80"/>
     </row>
     <row r="13" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="85"/>
+      <c r="A13" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="85">
+        <v>5</v>
+      </c>
       <c r="C13" s="81"/>
       <c r="D13" s="83"/>
-      <c r="E13" s="85"/>
+      <c r="E13" s="85">
+        <v>5</v>
+      </c>
       <c r="F13" s="81"/>
       <c r="G13" s="83"/>
-      <c r="H13" s="85"/>
+      <c r="H13" s="85">
+        <v>5</v>
+      </c>
       <c r="I13" s="81"/>
       <c r="J13" s="83"/>
       <c r="K13" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L13" s="81">
         <f t="shared" si="1"/>
@@ -1879,30 +1987,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N13" s="57" t="s">
+      <c r="N13" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O13" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="O13" s="57" t="s">
+      <c r="P13" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="P13" s="80"/>
     </row>
     <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="85"/>
+        <v>93</v>
+      </c>
+      <c r="B14" s="85">
+        <v>20</v>
+      </c>
       <c r="C14" s="81"/>
       <c r="D14" s="83"/>
-      <c r="E14" s="85"/>
+      <c r="E14" s="85">
+        <v>10</v>
+      </c>
       <c r="F14" s="81"/>
       <c r="G14" s="83"/>
-      <c r="H14" s="85"/>
+      <c r="H14" s="85">
+        <v>10</v>
+      </c>
       <c r="I14" s="81"/>
       <c r="J14" s="83"/>
       <c r="K14" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L14" s="81">
         <f t="shared" si="1"/>
@@ -1912,108 +2028,126 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N14" s="54" t="s">
+      <c r="N14" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O14" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="O14" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="P14" s="80"/>
+      <c r="P14" s="57" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>36</v>
+      <c r="A15" s="60" t="s">
+        <v>87</v>
       </c>
       <c r="B15" s="85">
-        <v>20</v>
-      </c>
-      <c r="C15" s="81">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C15" s="81"/>
       <c r="D15" s="83"/>
       <c r="E15" s="85">
-        <v>5</v>
-      </c>
-      <c r="F15" s="81">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F15" s="81"/>
       <c r="G15" s="83"/>
       <c r="H15" s="85">
-        <v>7</v>
-      </c>
-      <c r="I15" s="81">
-        <v>12</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I15" s="81"/>
       <c r="J15" s="83"/>
       <c r="K15" s="85">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L15" s="81">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="M15" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N15" s="54" t="s">
+      <c r="N15" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O15" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="O15" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="P15" s="80"/>
+      <c r="P15" s="57" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="81"/>
+      <c r="A16" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="85">
+        <v>20</v>
+      </c>
+      <c r="C16" s="81">
+        <v>20</v>
+      </c>
       <c r="D16" s="83"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="81"/>
+      <c r="E16" s="85">
+        <v>5</v>
+      </c>
+      <c r="F16" s="81">
+        <v>10</v>
+      </c>
       <c r="G16" s="83"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="81"/>
+      <c r="H16" s="85">
+        <v>7</v>
+      </c>
+      <c r="I16" s="81">
+        <v>12</v>
+      </c>
       <c r="J16" s="83"/>
       <c r="K16" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="L16" s="81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="M16" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N16" s="57" t="s">
+      <c r="N16" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O16" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="O16" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="P16" s="80"/>
+      <c r="P16" s="57" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="85"/>
+      <c r="A17" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="85">
+        <v>5</v>
+      </c>
       <c r="C17" s="81"/>
       <c r="D17" s="83"/>
-      <c r="E17" s="85"/>
+      <c r="E17" s="85">
+        <v>5</v>
+      </c>
       <c r="F17" s="81"/>
       <c r="G17" s="83"/>
-      <c r="H17" s="85"/>
+      <c r="H17" s="85">
+        <v>10</v>
+      </c>
       <c r="I17" s="81"/>
       <c r="J17" s="83"/>
       <c r="K17" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L17" s="81">
         <f t="shared" si="1"/>
@@ -2023,30 +2157,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N17" s="57" t="s">
+      <c r="N17" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O17" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="O17" s="57" t="s">
+      <c r="P17" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="P17" s="80"/>
     </row>
     <row r="18" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="85"/>
+        <v>72</v>
+      </c>
+      <c r="B18" s="85">
+        <v>5</v>
+      </c>
       <c r="C18" s="81"/>
       <c r="D18" s="83"/>
-      <c r="E18" s="85"/>
+      <c r="E18" s="85">
+        <v>5</v>
+      </c>
       <c r="F18" s="81"/>
       <c r="G18" s="83"/>
-      <c r="H18" s="85"/>
+      <c r="H18" s="85">
+        <v>10</v>
+      </c>
       <c r="I18" s="81"/>
       <c r="J18" s="83"/>
       <c r="K18" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L18" s="81">
         <f t="shared" si="1"/>
@@ -2056,30 +2198,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N18" s="57" t="s">
+      <c r="N18" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O18" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="O18" s="57" t="s">
+      <c r="P18" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="P18" s="80"/>
     </row>
     <row r="19" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="85"/>
+        <v>4</v>
+      </c>
+      <c r="B19" s="85">
+        <v>20</v>
+      </c>
       <c r="C19" s="81"/>
       <c r="D19" s="83"/>
-      <c r="E19" s="85"/>
+      <c r="E19" s="85">
+        <v>5</v>
+      </c>
       <c r="F19" s="81"/>
       <c r="G19" s="83"/>
-      <c r="H19" s="85"/>
+      <c r="H19" s="85">
+        <v>10</v>
+      </c>
       <c r="I19" s="81"/>
       <c r="J19" s="83"/>
       <c r="K19" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="L19" s="81">
         <f t="shared" si="1"/>
@@ -2089,30 +2239,38 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N19" s="57" t="s">
+      <c r="N19" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O19" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="O19" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="P19" s="80"/>
+      <c r="P19" s="54" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="20" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="85"/>
+        <v>51</v>
+      </c>
+      <c r="B20" s="85">
+        <v>40</v>
+      </c>
       <c r="C20" s="81"/>
       <c r="D20" s="83"/>
-      <c r="E20" s="85"/>
+      <c r="E20" s="85">
+        <v>10</v>
+      </c>
       <c r="F20" s="81"/>
       <c r="G20" s="83"/>
-      <c r="H20" s="85"/>
+      <c r="H20" s="85">
+        <v>9</v>
+      </c>
       <c r="I20" s="81"/>
       <c r="J20" s="83"/>
       <c r="K20" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="L20" s="81">
         <f t="shared" si="1"/>
@@ -2122,63 +2280,97 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N20" s="57" t="s">
+      <c r="N20" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O20" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="O20" s="54" t="s">
+      <c r="P20" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="P20" s="80"/>
     </row>
     <row r="21" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="85"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="83"/>
+        <v>145</v>
+      </c>
+      <c r="B21" s="85">
+        <v>40</v>
+      </c>
+      <c r="C21" s="81">
+        <v>40</v>
+      </c>
+      <c r="D21" s="83">
+        <v>45</v>
+      </c>
+      <c r="E21" s="85">
+        <v>10</v>
+      </c>
+      <c r="F21" s="81">
+        <v>10</v>
+      </c>
+      <c r="G21" s="83">
+        <v>7</v>
+      </c>
+      <c r="H21" s="85">
+        <v>12</v>
+      </c>
+      <c r="I21" s="81">
+        <v>15</v>
+      </c>
+      <c r="J21" s="83">
+        <v>10</v>
+      </c>
       <c r="K21" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="L21" s="81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="M21" s="83">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="57" t="s">
-        <v>138</v>
+        <v>62</v>
+      </c>
+      <c r="N21" s="80" t="s">
+        <v>203</v>
       </c>
       <c r="O21" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="P21" s="80"/>
+        <v>155</v>
+      </c>
+      <c r="P21" s="57" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="22" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="85"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="85">
+        <v>20</v>
+      </c>
       <c r="C22" s="81"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="85"/>
+      <c r="D22" s="83">
+        <v>30</v>
+      </c>
+      <c r="E22" s="85">
+        <v>10</v>
+      </c>
       <c r="F22" s="81"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="85"/>
+      <c r="G22" s="83">
+        <v>5</v>
+      </c>
+      <c r="H22" s="85">
+        <v>10</v>
+      </c>
       <c r="I22" s="81"/>
-      <c r="J22" s="83"/>
+      <c r="J22" s="83">
+        <v>7</v>
+      </c>
       <c r="K22" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L22" s="81">
         <f t="shared" si="1"/>
@@ -2186,28 +2378,30 @@
       </c>
       <c r="M22" s="83">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="N22" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O22" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="O22" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="P22" s="80"/>
+      <c r="P22" s="57" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
-        <v>145</v>
+        <v>69</v>
       </c>
       <c r="B23" s="85">
         <v>40</v>
       </c>
       <c r="C23" s="81">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D23" s="83">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E23" s="85">
         <v>10</v>
@@ -2216,435 +2410,296 @@
         <v>10</v>
       </c>
       <c r="G23" s="83">
+        <v>8</v>
+      </c>
+      <c r="H23" s="85">
+        <v>10</v>
+      </c>
+      <c r="I23" s="81">
         <v>7</v>
       </c>
-      <c r="H23" s="85">
-        <v>12</v>
-      </c>
-      <c r="I23" s="81">
-        <v>15</v>
-      </c>
       <c r="J23" s="83">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K23" s="85">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L23" s="81">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="M23" s="83">
         <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="N23" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="O23" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O23" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="P23" s="57" t="s">
         <v>183</v>
-      </c>
-      <c r="P23" s="80" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="85"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="83">
+      <c r="B24" s="85">
         <v>30</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="83">
+      <c r="C24" s="81">
+        <v>25</v>
+      </c>
+      <c r="D24" s="83"/>
+      <c r="E24" s="85">
         <v>5</v>
       </c>
-      <c r="H24" s="85"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="83">
-        <v>7</v>
-      </c>
+      <c r="F24" s="81">
+        <v>5</v>
+      </c>
+      <c r="G24" s="83"/>
+      <c r="H24" s="85">
+        <v>5</v>
+      </c>
+      <c r="I24" s="81">
+        <v>8</v>
+      </c>
+      <c r="J24" s="83"/>
       <c r="K24" s="85">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L24" s="81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="M24" s="83">
         <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="N24" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="O24" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="P24" s="80"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O24" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="P24" s="57" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="B25" s="85">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C25" s="81">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D25" s="83">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E25" s="85">
         <v>10</v>
       </c>
       <c r="F25" s="81">
+        <v>3</v>
+      </c>
+      <c r="G25" s="83">
         <v>10</v>
-      </c>
-      <c r="G25" s="83">
-        <v>8</v>
       </c>
       <c r="H25" s="85">
         <v>10</v>
       </c>
       <c r="I25" s="81">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J25" s="83">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K25" s="85">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L25" s="81">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="M25" s="83">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="N25" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O25" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="O25" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="P25" s="80" t="s">
-        <v>198</v>
+      <c r="P25" s="57" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
       <c r="B26" s="85">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C26" s="81">
-        <v>25</v>
-      </c>
-      <c r="D26" s="83"/>
+        <v>35</v>
+      </c>
+      <c r="D26" s="83">
+        <v>39</v>
+      </c>
       <c r="E26" s="85">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F26" s="81">
-        <v>5</v>
-      </c>
-      <c r="G26" s="83"/>
+        <v>10</v>
+      </c>
+      <c r="G26" s="83">
+        <v>7</v>
+      </c>
       <c r="H26" s="85">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I26" s="81">
-        <v>8</v>
-      </c>
-      <c r="J26" s="83"/>
+        <v>15</v>
+      </c>
+      <c r="J26" s="83">
+        <v>10</v>
+      </c>
       <c r="K26" s="85">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="L26" s="81">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="M26" s="83">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O26" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="O26" s="57" t="s">
+      <c r="P26" s="57" t="s">
         <v>181</v>
-      </c>
-      <c r="P26" s="80" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="85">
-        <v>10</v>
-      </c>
-      <c r="C27" s="81">
-        <v>27</v>
-      </c>
-      <c r="D27" s="83">
-        <v>10</v>
-      </c>
-      <c r="E27" s="85">
-        <v>10</v>
-      </c>
-      <c r="F27" s="81">
-        <v>3</v>
-      </c>
-      <c r="G27" s="83">
-        <v>10</v>
-      </c>
-      <c r="H27" s="85">
-        <v>10</v>
-      </c>
-      <c r="I27" s="81">
-        <v>10</v>
-      </c>
-      <c r="J27" s="83">
-        <v>10</v>
+        <v>196</v>
+      </c>
+      <c r="B27" s="84" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="82" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="84" t="s">
+        <v>190</v>
+      </c>
+      <c r="F27" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="82" t="s">
+        <v>131</v>
+      </c>
+      <c r="H27" s="84" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="J27" s="82" t="s">
+        <v>131</v>
       </c>
       <c r="K27" s="85">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="L27" s="81">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M27" s="83">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="N27" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="O27" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="P27" s="80" t="s">
-        <v>198</v>
+        <v>40</v>
+      </c>
+      <c r="N27" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O27" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="P27" s="57" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="85">
-        <v>40</v>
-      </c>
-      <c r="C28" s="81">
-        <v>43</v>
-      </c>
-      <c r="D28" s="83">
-        <v>45</v>
-      </c>
-      <c r="E28" s="85">
-        <v>15</v>
-      </c>
-      <c r="F28" s="81">
-        <v>12</v>
-      </c>
-      <c r="G28" s="83">
-        <v>8</v>
-      </c>
-      <c r="H28" s="85">
-        <v>12</v>
-      </c>
-      <c r="I28" s="81">
-        <v>15</v>
-      </c>
-      <c r="J28" s="83">
-        <v>9</v>
+      <c r="A28" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="84" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="82" t="s">
+        <v>199</v>
+      </c>
+      <c r="E28" s="84" t="s">
+        <v>190</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="H28" s="84" t="s">
+        <v>190</v>
+      </c>
+      <c r="I28" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="82" t="s">
+        <v>190</v>
       </c>
       <c r="K28" s="85">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="L28" s="81">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="M28" s="83">
         <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="N28" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="O28" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="P28" s="80" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="B29" s="85">
-        <v>35</v>
-      </c>
-      <c r="C29" s="81">
-        <v>35</v>
-      </c>
-      <c r="D29" s="83">
-        <v>39</v>
-      </c>
-      <c r="E29" s="85">
-        <v>12</v>
-      </c>
-      <c r="F29" s="81">
-        <v>10</v>
-      </c>
-      <c r="G29" s="83">
-        <v>7</v>
-      </c>
-      <c r="H29" s="85">
-        <v>10</v>
-      </c>
-      <c r="I29" s="81">
-        <v>15</v>
-      </c>
-      <c r="J29" s="83">
-        <v>10</v>
-      </c>
-      <c r="K29" s="85">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="L29" s="81">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="M29" s="83">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-      <c r="N29" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="O29" s="57" t="s">
-        <v>181</v>
-      </c>
-      <c r="P29" s="80" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
-        <v>196</v>
-      </c>
-      <c r="B30" s="84" t="s">
-        <v>191</v>
-      </c>
-      <c r="C30" s="53" t="s">
-        <v>191</v>
-      </c>
-      <c r="D30" s="82" t="s">
-        <v>191</v>
-      </c>
-      <c r="E30" s="84" t="s">
-        <v>190</v>
-      </c>
-      <c r="F30" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="82" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" s="84" t="s">
-        <v>189</v>
-      </c>
-      <c r="I30" s="53" t="s">
-        <v>190</v>
-      </c>
-      <c r="J30" s="82" t="s">
-        <v>131</v>
-      </c>
-      <c r="K30" s="85">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="L30" s="81">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="M30" s="83">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="N30" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="N28" s="80" t="s">
+        <v>203</v>
+      </c>
+      <c r="O28" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="O30" s="57" t="s">
+      <c r="P28" s="57" t="s">
         <v>183</v>
-      </c>
-      <c r="P30" s="80" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="84"/>
-      <c r="C31" s="53" t="s">
-        <v>197</v>
-      </c>
-      <c r="D31" s="82" t="s">
-        <v>199</v>
-      </c>
-      <c r="E31" s="84"/>
-      <c r="F31" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="G31" s="82" t="s">
-        <v>165</v>
-      </c>
-      <c r="H31" s="84"/>
-      <c r="I31" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="J31" s="82" t="s">
-        <v>190</v>
-      </c>
-      <c r="K31" s="85">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="81">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="M31" s="83">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="N31" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="O31" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="P31" s="80" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2665,7 +2720,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G21"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3662,26 +3717,26 @@
       <c r="B1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="88"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="87" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="88"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="87" t="s">
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="88" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="88"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="87" t="s">
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="90"/>
       <c r="O1" s="79"/>
       <c r="P1" s="79"/>
       <c r="Q1" s="79"/>

</xml_diff>